<commit_message>
refactor: rename SpecialSpeaker to SpecialName and update related references fix: change translate_type to validate_type in background and camera generators fix: update speaker references to character_name in text generators chore: add icon and update Excel files
</commit_message>
<xml_diff>
--- a/param_config/param_data_renpy.xlsx
+++ b/param_config/param_data_renpy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\视觉小说项目\【表格演出工具】git仓库\param_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23DB856-A10C-4A89-A65D-CFB6C86683CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816F361F-F5F1-4D32-86F0-5B5CF3789950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>

</xml_diff>